<commit_message>
Basic Webserver, airplane updates, and basic controller
The controller and webserver are not communicating as of yet
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Item</t>
   </si>
@@ -68,13 +68,19 @@
     <t>Female/male jumper wires</t>
   </si>
   <si>
-    <t>9-DOF board</t>
-  </si>
-  <si>
-    <t>Feather M0 LoRa</t>
-  </si>
-  <si>
-    <t>RFM95W</t>
+    <t>COST IS IN USD</t>
+  </si>
+  <si>
+    <t>Foam board</t>
+  </si>
+  <si>
+    <t>9-DOF board (Gyro, accel, mag)</t>
+  </si>
+  <si>
+    <t>Feather M0 LoRa (Arduino)</t>
+  </si>
+  <si>
+    <t>RFM95W (Radio)</t>
   </si>
 </sst>
 </file>
@@ -430,15 +436,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B24768-C628-44C7-BA7A-7E6463FE83D8}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,8 +461,11 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -467,7 +480,7 @@
         <v>22.39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -478,11 +491,11 @@
         <v>2.96</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D14" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D15" si="0">B3*C3</f>
         <v>2.96</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -497,7 +510,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -512,7 +525,7 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -527,7 +540,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -542,7 +555,7 @@
         <v>32.840000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -557,7 +570,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -572,7 +585,7 @@
         <v>39.950000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -587,7 +600,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -602,9 +615,9 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -617,9 +630,9 @@
         <v>14.95</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -632,9 +645,9 @@
         <v>34.950000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -647,10 +660,25 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.5</v>
+      </c>
       <c r="D15" s="1">
-        <f>SUM(D2:D14)</f>
-        <v>185.47000000000003</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <f>SUM(D2:D15)</f>
+        <v>191.47000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>